<commit_message>
Results, tables, and figures
Added the results section, and our tables and figures should we need
them for the analysis.
</commit_message>
<xml_diff>
--- a/Faraday Lab data tables.xlsx
+++ b/Faraday Lab data tables.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="-210" yWindow="75" windowWidth="20730" windowHeight="11760" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="changeCurrentData" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>Theta rel</t>
   </si>
@@ -81,16 +81,7 @@
     <t>error c</t>
   </si>
   <si>
-    <t>0.0088553 +/- 0.0010</t>
-  </si>
-  <si>
-    <t>c1 = 0.030849 +/- 0.0014</t>
-  </si>
-  <si>
-    <t>c2 = 0.049599 +/- 0.0013</t>
-  </si>
-  <si>
-    <t>c3 = 0.072754 +/- 0.0015</t>
+    <t>I (A)</t>
   </si>
 </sst>
 </file>
@@ -135,6 +126,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -466,9 +462,9 @@
       <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -497,7 +493,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -526,7 +522,7 @@
         <v>2.8679999999999999E-12</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0.17453299999999999</v>
       </c>
@@ -555,7 +551,7 @@
         <v>7.2929999999999997E-12</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0.34906599999999999</v>
       </c>
@@ -584,7 +580,7 @@
         <v>3.5739999999999998E-11</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0.52359900000000004</v>
       </c>
@@ -613,7 +609,7 @@
         <v>9.5590000000000003E-11</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0.69813199999999997</v>
       </c>
@@ -642,7 +638,7 @@
         <v>3.1599999999999999E-12</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0.87266500000000002</v>
       </c>
@@ -671,7 +667,7 @@
         <v>7.4260000000000001E-12</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1.0471999999999999</v>
       </c>
@@ -700,7 +696,7 @@
         <v>4.1169999999999998E-11</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1.22173</v>
       </c>
@@ -729,7 +725,7 @@
         <v>6.0210000000000005E-11</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1.3962600000000001</v>
       </c>
@@ -758,7 +754,7 @@
         <v>9.1640000000000006E-11</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1.5708</v>
       </c>
@@ -787,7 +783,7 @@
         <v>1.048E-10</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1.74533</v>
       </c>
@@ -816,7 +812,7 @@
         <v>1.8179999999999999E-11</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1.9198599999999999</v>
       </c>
@@ -845,7 +841,7 @@
         <v>2.449E-10</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2.0943999999999998</v>
       </c>
@@ -874,7 +870,7 @@
         <v>8.081E-12</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2.2689300000000001</v>
       </c>
@@ -903,7 +899,7 @@
         <v>9.2440000000000003E-10</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2.44346</v>
       </c>
@@ -932,7 +928,7 @@
         <v>1.043E-10</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2.6179899999999998</v>
       </c>
@@ -961,7 +957,7 @@
         <v>2.4070000000000001E-11</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2.7925300000000002</v>
       </c>
@@ -990,7 +986,7 @@
         <v>3.0290000000000001E-12</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2.96706</v>
       </c>
@@ -1019,7 +1015,7 @@
         <v>7.2089999999999999E-13</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>3.1415899999999999</v>
       </c>
@@ -1048,7 +1044,7 @@
         <v>2.9670000000000002E-12</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>3.3161299999999998</v>
       </c>
@@ -1077,7 +1073,7 @@
         <v>1.8350000000000002E-12</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>3.4906600000000001</v>
       </c>
@@ -1106,7 +1102,7 @@
         <v>8.3750000000000002E-12</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>3.6651899999999999</v>
       </c>
@@ -1135,7 +1131,7 @@
         <v>1.96E-10</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>3.8397199999999998</v>
       </c>
@@ -1164,7 +1160,7 @@
         <v>1.5680000000000001E-11</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>4.0142600000000002</v>
       </c>
@@ -1193,7 +1189,7 @@
         <v>4.089E-12</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>4.18879</v>
       </c>
@@ -1222,7 +1218,7 @@
         <v>3.7209999999999999E-10</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>4.3633199999999999</v>
       </c>
@@ -1251,7 +1247,7 @@
         <v>1.448E-11</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>4.5378600000000002</v>
       </c>
@@ -1280,7 +1276,7 @@
         <v>4.9490000000000002E-10</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>4.7123900000000001</v>
       </c>
@@ -1309,7 +1305,7 @@
         <v>1.9369999999999999E-10</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>4.8869199999999999</v>
       </c>
@@ -1338,7 +1334,7 @@
         <v>3.8649999999999997E-11</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>5.0614499999999998</v>
       </c>
@@ -1367,7 +1363,7 @@
         <v>2.0339999999999999E-10</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>5.2359900000000001</v>
       </c>
@@ -1396,7 +1392,7 @@
         <v>3.3339999999999998E-11</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>5.41052</v>
       </c>
@@ -1425,7 +1421,7 @@
         <v>9.3340000000000004E-13</v>
       </c>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>5.5850499999999998</v>
       </c>
@@ -1454,7 +1450,7 @@
         <v>5.325E-12</v>
       </c>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>5.7595900000000002</v>
       </c>
@@ -1483,7 +1479,7 @@
         <v>6.64E-12</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>5.9341200000000001</v>
       </c>
@@ -1512,7 +1508,7 @@
         <v>7.8750000000000003E-12</v>
       </c>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>6.1086499999999999</v>
       </c>
@@ -1555,13 +1551,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.75" customWidth="1"/>
+    <col min="2" max="2" width="17.25" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -1575,7 +1575,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1589,7 +1589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2.1999999999999999E-2</v>
       </c>
@@ -1603,7 +1603,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4.07E-2</v>
       </c>
@@ -1617,7 +1617,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>6.3899999999999998E-2</v>
       </c>
@@ -1643,208 +1643,250 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
         <v>13</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>14</v>
       </c>
-      <c r="C1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>-3</v>
+      </c>
+      <c r="B2">
+        <v>-323</v>
+      </c>
+      <c r="C2">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2">
+      <c r="D2">
         <v>2.8220000000000001</v>
       </c>
-      <c r="B2" s="1">
+      <c r="E2" s="1">
         <v>1.296E-10</v>
       </c>
-      <c r="C2">
-        <v>-323</v>
-      </c>
-      <c r="D2">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
+        <v>-2.5</v>
+      </c>
+      <c r="B3">
+        <v>-269</v>
+      </c>
+      <c r="C3">
+        <v>10</v>
+      </c>
+      <c r="D3">
         <v>2.887</v>
       </c>
-      <c r="B3" s="1">
+      <c r="E3" s="1">
         <v>5.4699999999999997E-10</v>
       </c>
-      <c r="C3">
-        <v>-269</v>
-      </c>
-      <c r="D3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
+        <v>-2</v>
+      </c>
+      <c r="B4">
+        <v>-215</v>
+      </c>
+      <c r="C4">
+        <v>8</v>
+      </c>
+      <c r="D4">
         <v>2.9510000000000001</v>
       </c>
-      <c r="B4" s="1">
+      <c r="E4" s="1">
         <v>3.7220000000000002E-10</v>
       </c>
-      <c r="C4">
-        <v>-215</v>
-      </c>
-      <c r="D4">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
+        <v>-1.5</v>
+      </c>
+      <c r="B5">
+        <v>-161</v>
+      </c>
+      <c r="C5">
+        <v>6</v>
+      </c>
+      <c r="D5">
         <v>3.016</v>
       </c>
-      <c r="B5" s="1">
+      <c r="E5" s="1">
         <v>3.7749999999999999E-11</v>
       </c>
-      <c r="C5">
-        <v>-161</v>
-      </c>
-      <c r="D5">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
+        <v>-1</v>
+      </c>
+      <c r="B6">
+        <v>-108</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6">
         <v>3.0819999999999999</v>
       </c>
-      <c r="B6" s="1">
+      <c r="E6" s="1">
         <v>8.98E-10</v>
       </c>
-      <c r="C6">
-        <v>-108</v>
-      </c>
-      <c r="D6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
+        <v>-0.5</v>
+      </c>
+      <c r="B7">
+        <v>-54</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
         <v>3.145</v>
       </c>
-      <c r="B7" s="1">
+      <c r="E7" s="1">
         <v>9.034E-10</v>
       </c>
-      <c r="C7">
-        <v>-54</v>
-      </c>
-      <c r="D7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>3.2109999999999999</v>
-      </c>
-      <c r="B8" s="1">
-        <v>1.184E-9</v>
+        <v>0</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
       <c r="D8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+        <v>3.2109999999999999</v>
+      </c>
+      <c r="E8" s="1">
+        <v>1.184E-9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
+        <v>0.5</v>
+      </c>
+      <c r="B9">
+        <v>54</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9">
         <v>3.2719999999999998</v>
       </c>
-      <c r="B9" s="1">
+      <c r="E9" s="1">
         <v>1.161E-10</v>
       </c>
-      <c r="C9">
-        <v>54</v>
-      </c>
-      <c r="D9">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10">
+        <v>108</v>
+      </c>
+      <c r="C10">
+        <v>4</v>
+      </c>
+      <c r="D10">
+        <v>3.3380000000000001</v>
+      </c>
+      <c r="E10" s="1">
+        <v>2.0510000000000001E-9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1.5</v>
+      </c>
+      <c r="B11">
+        <v>161</v>
+      </c>
+      <c r="C11">
+        <v>6</v>
+      </c>
+      <c r="D11">
+        <v>3.4039999999999999</v>
+      </c>
+      <c r="E11" s="1">
+        <v>2.133E-9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10">
-        <v>3.3380000000000001</v>
-      </c>
-      <c r="B10" s="1">
-        <v>2.0510000000000001E-9</v>
-      </c>
-      <c r="C10">
-        <v>108</v>
-      </c>
-      <c r="D10">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11">
-        <v>3.4039999999999999</v>
-      </c>
-      <c r="B11" s="1">
-        <v>2.133E-9</v>
-      </c>
-      <c r="C11">
-        <v>161</v>
-      </c>
-      <c r="D11">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12">
+      <c r="B12">
+        <v>215</v>
+      </c>
+      <c r="C12">
+        <v>8</v>
+      </c>
+      <c r="D12">
         <v>3.468</v>
       </c>
-      <c r="B12" s="1">
+      <c r="E12" s="1">
         <v>6.9580000000000002E-10</v>
       </c>
-      <c r="C12">
-        <v>215</v>
-      </c>
-      <c r="D12">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
+        <v>2.5</v>
+      </c>
+      <c r="B13">
+        <v>269</v>
+      </c>
+      <c r="C13">
+        <v>10</v>
+      </c>
+      <c r="D13">
         <v>3.5339999999999998</v>
       </c>
-      <c r="B13" s="1">
+      <c r="E13" s="1">
         <v>1.1160000000000001E-9</v>
       </c>
-      <c r="C13">
-        <v>269</v>
-      </c>
-      <c r="D13">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
+        <v>3</v>
+      </c>
+      <c r="B14">
+        <v>323</v>
+      </c>
+      <c r="C14">
+        <v>12</v>
+      </c>
+      <c r="D14">
         <v>3.5990000000000002</v>
       </c>
-      <c r="B14" s="1">
+      <c r="E14" s="1">
         <v>1.045E-9</v>
-      </c>
-      <c r="C14">
-        <v>323</v>
-      </c>
-      <c r="D14">
-        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -1859,20 +1901,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -1883,7 +1925,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -1894,7 +1936,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1905,7 +1947,7 @@
         <v>1.4E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -1916,7 +1958,7 @@
         <v>1.2999999999999999E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
@@ -1925,26 +1967,6 @@
       </c>
       <c r="C6">
         <v>1.5E-3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="E7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="E8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="E9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="E10" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated graphics and excel file
more readable plots and diagrams, organized excel file.
</commit_message>
<xml_diff>
--- a/Faraday Lab data tables.xlsx
+++ b/Faraday Lab data tables.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-210" yWindow="75" windowWidth="20730" windowHeight="11760" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="1380" yWindow="460" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="changeCurrentData" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="ChangeThetaRaw" sheetId="1" r:id="rId1"/>
+    <sheet name="changeThetaCalculations" sheetId="2" r:id="rId2"/>
+    <sheet name="changeCurrent" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -88,10 +87,26 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -114,14 +129,38 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="13">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -462,9 +501,9 @@
       <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -493,7 +532,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2">
         <v>0</v>
       </c>
@@ -522,7 +561,7 @@
         <v>2.8679999999999999E-12</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
       <c r="A3">
         <v>0.17453299999999999</v>
       </c>
@@ -551,7 +590,7 @@
         <v>7.2929999999999997E-12</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9">
       <c r="A4">
         <v>0.34906599999999999</v>
       </c>
@@ -580,7 +619,7 @@
         <v>3.5739999999999998E-11</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9">
       <c r="A5">
         <v>0.52359900000000004</v>
       </c>
@@ -609,7 +648,7 @@
         <v>9.5590000000000003E-11</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9">
       <c r="A6">
         <v>0.69813199999999997</v>
       </c>
@@ -638,7 +677,7 @@
         <v>3.1599999999999999E-12</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9">
       <c r="A7">
         <v>0.87266500000000002</v>
       </c>
@@ -667,7 +706,7 @@
         <v>7.4260000000000001E-12</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9">
       <c r="A8">
         <v>1.0471999999999999</v>
       </c>
@@ -696,7 +735,7 @@
         <v>4.1169999999999998E-11</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9">
       <c r="A9">
         <v>1.22173</v>
       </c>
@@ -725,7 +764,7 @@
         <v>6.0210000000000005E-11</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9">
       <c r="A10">
         <v>1.3962600000000001</v>
       </c>
@@ -754,7 +793,7 @@
         <v>9.1640000000000006E-11</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9">
       <c r="A11">
         <v>1.5708</v>
       </c>
@@ -783,7 +822,7 @@
         <v>1.048E-10</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9">
       <c r="A12">
         <v>1.74533</v>
       </c>
@@ -812,7 +851,7 @@
         <v>1.8179999999999999E-11</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9">
       <c r="A13">
         <v>1.9198599999999999</v>
       </c>
@@ -841,7 +880,7 @@
         <v>2.449E-10</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9">
       <c r="A14">
         <v>2.0943999999999998</v>
       </c>
@@ -870,7 +909,7 @@
         <v>8.081E-12</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9">
       <c r="A15">
         <v>2.2689300000000001</v>
       </c>
@@ -899,7 +938,7 @@
         <v>9.2440000000000003E-10</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9">
       <c r="A16">
         <v>2.44346</v>
       </c>
@@ -928,7 +967,7 @@
         <v>1.043E-10</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9">
       <c r="A17">
         <v>2.6179899999999998</v>
       </c>
@@ -957,7 +996,7 @@
         <v>2.4070000000000001E-11</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9">
       <c r="A18">
         <v>2.7925300000000002</v>
       </c>
@@ -986,7 +1025,7 @@
         <v>3.0290000000000001E-12</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9">
       <c r="A19">
         <v>2.96706</v>
       </c>
@@ -1015,7 +1054,7 @@
         <v>7.2089999999999999E-13</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9">
       <c r="A20">
         <v>3.1415899999999999</v>
       </c>
@@ -1044,7 +1083,7 @@
         <v>2.9670000000000002E-12</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9">
       <c r="A21">
         <v>3.3161299999999998</v>
       </c>
@@ -1073,7 +1112,7 @@
         <v>1.8350000000000002E-12</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9">
       <c r="A22">
         <v>3.4906600000000001</v>
       </c>
@@ -1102,7 +1141,7 @@
         <v>8.3750000000000002E-12</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9">
       <c r="A23">
         <v>3.6651899999999999</v>
       </c>
@@ -1131,7 +1170,7 @@
         <v>1.96E-10</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9">
       <c r="A24">
         <v>3.8397199999999998</v>
       </c>
@@ -1160,7 +1199,7 @@
         <v>1.5680000000000001E-11</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9">
       <c r="A25">
         <v>4.0142600000000002</v>
       </c>
@@ -1189,7 +1228,7 @@
         <v>4.089E-12</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9">
       <c r="A26">
         <v>4.18879</v>
       </c>
@@ -1218,7 +1257,7 @@
         <v>3.7209999999999999E-10</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9">
       <c r="A27">
         <v>4.3633199999999999</v>
       </c>
@@ -1247,7 +1286,7 @@
         <v>1.448E-11</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9">
       <c r="A28">
         <v>4.5378600000000002</v>
       </c>
@@ -1276,7 +1315,7 @@
         <v>4.9490000000000002E-10</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9">
       <c r="A29">
         <v>4.7123900000000001</v>
       </c>
@@ -1305,7 +1344,7 @@
         <v>1.9369999999999999E-10</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9">
       <c r="A30">
         <v>4.8869199999999999</v>
       </c>
@@ -1334,7 +1373,7 @@
         <v>3.8649999999999997E-11</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9">
       <c r="A31">
         <v>5.0614499999999998</v>
       </c>
@@ -1363,7 +1402,7 @@
         <v>2.0339999999999999E-10</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9">
       <c r="A32">
         <v>5.2359900000000001</v>
       </c>
@@ -1392,7 +1431,7 @@
         <v>3.3339999999999998E-11</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9">
       <c r="A33">
         <v>5.41052</v>
       </c>
@@ -1421,7 +1460,7 @@
         <v>9.3340000000000004E-13</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9">
       <c r="A34">
         <v>5.5850499999999998</v>
       </c>
@@ -1450,7 +1489,7 @@
         <v>5.325E-12</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9">
       <c r="A35">
         <v>5.7595900000000002</v>
       </c>
@@ -1479,7 +1518,7 @@
         <v>6.64E-12</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9">
       <c r="A36">
         <v>5.9341200000000001</v>
       </c>
@@ -1508,7 +1547,7 @@
         <v>7.8750000000000003E-12</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9">
       <c r="A37">
         <v>6.1086499999999999</v>
       </c>
@@ -1549,90 +1588,141 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="16.75" customWidth="1"/>
-    <col min="2" max="2" width="17.25" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="2" max="2" width="17.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
         <v>9</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
         <v>10</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3">
         <v>0</v>
       </c>
-      <c r="B2">
+      <c r="B3">
         <v>2E-3</v>
       </c>
-      <c r="C2">
+      <c r="C3">
         <v>0</v>
       </c>
-      <c r="D2">
+      <c r="D3">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>8.8553E-3</v>
+      </c>
+      <c r="G3">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="B3">
+      <c r="B4">
         <v>2.3999999999999998E-3</v>
       </c>
-      <c r="C3">
+      <c r="C4">
         <v>108</v>
       </c>
-      <c r="D3">
+      <c r="D4">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>3.0849000000000001E-2</v>
+      </c>
+      <c r="G4">
+        <v>1.4E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5">
         <v>4.07E-2</v>
       </c>
-      <c r="B4">
+      <c r="B5">
         <v>2.3E-3</v>
       </c>
-      <c r="C4">
+      <c r="C5">
         <v>215</v>
       </c>
-      <c r="D4">
+      <c r="D5">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <v>4.9598999999999997E-2</v>
+      </c>
+      <c r="G5">
+        <v>1.2999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6">
         <v>6.3899999999999998E-2</v>
       </c>
-      <c r="B5">
+      <c r="B6">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="C5">
+      <c r="C6">
         <v>323</v>
       </c>
-      <c r="D5">
+      <c r="D6">
         <v>12</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
+      <c r="F6">
+        <v>7.2753999999999999E-2</v>
+      </c>
+      <c r="G6">
+        <v>1.5E-3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1649,9 +1739,9 @@
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -1668,7 +1758,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>-3</v>
       </c>
@@ -1685,7 +1775,7 @@
         <v>1.296E-10</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>-2.5</v>
       </c>
@@ -1702,7 +1792,7 @@
         <v>5.4699999999999997E-10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>-2</v>
       </c>
@@ -1719,7 +1809,7 @@
         <v>3.7220000000000002E-10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>-1.5</v>
       </c>
@@ -1736,7 +1826,7 @@
         <v>3.7749999999999999E-11</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>-1</v>
       </c>
@@ -1753,7 +1843,7 @@
         <v>8.98E-10</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7">
         <v>-0.5</v>
       </c>
@@ -1770,7 +1860,7 @@
         <v>9.034E-10</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8">
         <v>0</v>
       </c>
@@ -1787,7 +1877,7 @@
         <v>1.184E-9</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9">
         <v>0.5</v>
       </c>
@@ -1804,7 +1894,7 @@
         <v>1.161E-10</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1821,7 +1911,7 @@
         <v>2.0510000000000001E-9</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11">
         <v>1.5</v>
       </c>
@@ -1838,7 +1928,7 @@
         <v>2.133E-9</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12">
         <v>2</v>
       </c>
@@ -1855,7 +1945,7 @@
         <v>6.9580000000000002E-10</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13">
         <v>2.5</v>
       </c>
@@ -1872,7 +1962,7 @@
         <v>1.1160000000000001E-9</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14">
         <v>3</v>
       </c>
@@ -1887,86 +1977,6 @@
       </c>
       <c r="E14" s="1">
         <v>1.045E-9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>0</v>
-      </c>
-      <c r="B3">
-        <v>8.8553E-3</v>
-      </c>
-      <c r="C3">
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4">
-        <v>3.0849000000000001E-2</v>
-      </c>
-      <c r="C4">
-        <v>1.4E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>2</v>
-      </c>
-      <c r="B5">
-        <v>4.9598999999999997E-2</v>
-      </c>
-      <c r="C5">
-        <v>1.2999999999999999E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>3</v>
-      </c>
-      <c r="B6">
-        <v>7.2753999999999999E-2</v>
-      </c>
-      <c r="C6">
-        <v>1.5E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated plots and diagram
</commit_message>
<xml_diff>
--- a/Faraday Lab data tables.xlsx
+++ b/Faraday Lab data tables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1380" yWindow="460" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="1380" yWindow="460" windowWidth="19140" windowHeight="16140" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="ChangeThetaRaw" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>Theta rel</t>
   </si>
@@ -74,13 +74,31 @@
     <t>current</t>
   </si>
   <si>
-    <t>c value</t>
-  </si>
-  <si>
     <t>error c</t>
   </si>
   <si>
     <t>I (A)</t>
+  </si>
+  <si>
+    <t>dB</t>
+  </si>
+  <si>
+    <t>B*L (mTcm)</t>
+  </si>
+  <si>
+    <t>c value (rad)</t>
+  </si>
+  <si>
+    <t>B (mT)</t>
+  </si>
+  <si>
+    <t>field for 2A measured</t>
+  </si>
+  <si>
+    <t>fields and errors for 1 and 3 A extrapolated from this measurement given expected proportionality between current and field</t>
+  </si>
+  <si>
+    <t>Theta rel actual (rad)</t>
   </si>
 </sst>
 </file>
@@ -144,9 +162,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -495,15 +516,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="10" max="10" width="19.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -531,8 +555,11 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="J1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2">
         <v>0</v>
       </c>
@@ -560,8 +587,12 @@
       <c r="I2" s="1">
         <v>2.8679999999999999E-12</v>
       </c>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="J2">
+        <f>A2-(3.141592/2)</f>
+        <v>-1.5707960000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3">
         <v>0.17453299999999999</v>
       </c>
@@ -589,8 +620,12 @@
       <c r="I3" s="1">
         <v>7.2929999999999997E-12</v>
       </c>
-    </row>
-    <row r="4" spans="1:9">
+      <c r="J3">
+        <f t="shared" ref="J3:J37" si="0">A3-(3.141592/2)</f>
+        <v>-1.396263</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4">
         <v>0.34906599999999999</v>
       </c>
@@ -618,8 +653,12 @@
       <c r="I4" s="1">
         <v>3.5739999999999998E-11</v>
       </c>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="J4">
+        <f t="shared" si="0"/>
+        <v>-1.22173</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5">
         <v>0.52359900000000004</v>
       </c>
@@ -647,8 +686,12 @@
       <c r="I5" s="1">
         <v>9.5590000000000003E-11</v>
       </c>
-    </row>
-    <row r="6" spans="1:9">
+      <c r="J5">
+        <f t="shared" si="0"/>
+        <v>-1.0471970000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6">
         <v>0.69813199999999997</v>
       </c>
@@ -676,8 +719,12 @@
       <c r="I6" s="1">
         <v>3.1599999999999999E-12</v>
       </c>
-    </row>
-    <row r="7" spans="1:9">
+      <c r="J6">
+        <f t="shared" si="0"/>
+        <v>-0.87266400000000011</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7">
         <v>0.87266500000000002</v>
       </c>
@@ -705,8 +752,12 @@
       <c r="I7" s="1">
         <v>7.4260000000000001E-12</v>
       </c>
-    </row>
-    <row r="8" spans="1:9">
+      <c r="J7">
+        <f t="shared" si="0"/>
+        <v>-0.69813100000000006</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8">
         <v>1.0471999999999999</v>
       </c>
@@ -734,8 +785,12 @@
       <c r="I8" s="1">
         <v>4.1169999999999998E-11</v>
       </c>
-    </row>
-    <row r="9" spans="1:9">
+      <c r="J8">
+        <f t="shared" si="0"/>
+        <v>-0.52359600000000017</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9">
         <v>1.22173</v>
       </c>
@@ -763,8 +818,12 @@
       <c r="I9" s="1">
         <v>6.0210000000000005E-11</v>
       </c>
-    </row>
-    <row r="10" spans="1:9">
+      <c r="J9">
+        <f t="shared" si="0"/>
+        <v>-0.3490660000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10">
         <v>1.3962600000000001</v>
       </c>
@@ -792,8 +851,12 @@
       <c r="I10" s="1">
         <v>9.1640000000000006E-11</v>
       </c>
-    </row>
-    <row r="11" spans="1:9">
+      <c r="J10">
+        <f t="shared" si="0"/>
+        <v>-0.17453600000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11">
         <v>1.5708</v>
       </c>
@@ -821,8 +884,12 @@
       <c r="I11" s="1">
         <v>1.048E-10</v>
       </c>
-    </row>
-    <row r="12" spans="1:9">
+      <c r="J11">
+        <f t="shared" si="0"/>
+        <v>3.9999999998929781E-6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12">
         <v>1.74533</v>
       </c>
@@ -850,8 +917,12 @@
       <c r="I12" s="1">
         <v>1.8179999999999999E-11</v>
       </c>
-    </row>
-    <row r="13" spans="1:9">
+      <c r="J12">
+        <f t="shared" si="0"/>
+        <v>0.17453399999999997</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13">
         <v>1.9198599999999999</v>
       </c>
@@ -879,8 +950,12 @@
       <c r="I13" s="1">
         <v>2.449E-10</v>
       </c>
-    </row>
-    <row r="14" spans="1:9">
+      <c r="J13">
+        <f t="shared" si="0"/>
+        <v>0.34906399999999982</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14">
         <v>2.0943999999999998</v>
       </c>
@@ -908,8 +983,12 @@
       <c r="I14" s="1">
         <v>8.081E-12</v>
       </c>
-    </row>
-    <row r="15" spans="1:9">
+      <c r="J14">
+        <f t="shared" si="0"/>
+        <v>0.52360399999999974</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15">
         <v>2.2689300000000001</v>
       </c>
@@ -937,8 +1016,12 @@
       <c r="I15" s="1">
         <v>9.2440000000000003E-10</v>
       </c>
-    </row>
-    <row r="16" spans="1:9">
+      <c r="J15">
+        <f t="shared" si="0"/>
+        <v>0.69813400000000003</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16">
         <v>2.44346</v>
       </c>
@@ -966,8 +1049,12 @@
       <c r="I16" s="1">
         <v>1.043E-10</v>
       </c>
-    </row>
-    <row r="17" spans="1:9">
+      <c r="J16">
+        <f t="shared" si="0"/>
+        <v>0.87266399999999988</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17">
         <v>2.6179899999999998</v>
       </c>
@@ -995,8 +1082,12 @@
       <c r="I17" s="1">
         <v>2.4070000000000001E-11</v>
       </c>
-    </row>
-    <row r="18" spans="1:9">
+      <c r="J17">
+        <f t="shared" si="0"/>
+        <v>1.0471939999999997</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18">
         <v>2.7925300000000002</v>
       </c>
@@ -1024,8 +1115,12 @@
       <c r="I18" s="1">
         <v>3.0290000000000001E-12</v>
       </c>
-    </row>
-    <row r="19" spans="1:9">
+      <c r="J18">
+        <f t="shared" si="0"/>
+        <v>1.2217340000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19">
         <v>2.96706</v>
       </c>
@@ -1053,8 +1148,12 @@
       <c r="I19" s="1">
         <v>7.2089999999999999E-13</v>
       </c>
-    </row>
-    <row r="20" spans="1:9">
+      <c r="J19">
+        <f t="shared" si="0"/>
+        <v>1.3962639999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20">
         <v>3.1415899999999999</v>
       </c>
@@ -1082,8 +1181,12 @@
       <c r="I20" s="1">
         <v>2.9670000000000002E-12</v>
       </c>
-    </row>
-    <row r="21" spans="1:9">
+      <c r="J20">
+        <f t="shared" si="0"/>
+        <v>1.5707939999999998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21">
         <v>3.3161299999999998</v>
       </c>
@@ -1111,8 +1214,12 @@
       <c r="I21" s="1">
         <v>1.8350000000000002E-12</v>
       </c>
-    </row>
-    <row r="22" spans="1:9">
+      <c r="J21">
+        <f t="shared" si="0"/>
+        <v>1.7453339999999997</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
       <c r="A22">
         <v>3.4906600000000001</v>
       </c>
@@ -1140,8 +1247,12 @@
       <c r="I22" s="1">
         <v>8.3750000000000002E-12</v>
       </c>
-    </row>
-    <row r="23" spans="1:9">
+      <c r="J22">
+        <f t="shared" si="0"/>
+        <v>1.919864</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
       <c r="A23">
         <v>3.6651899999999999</v>
       </c>
@@ -1169,8 +1280,12 @@
       <c r="I23" s="1">
         <v>1.96E-10</v>
       </c>
-    </row>
-    <row r="24" spans="1:9">
+      <c r="J23">
+        <f t="shared" si="0"/>
+        <v>2.0943939999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
       <c r="A24">
         <v>3.8397199999999998</v>
       </c>
@@ -1198,8 +1313,12 @@
       <c r="I24" s="1">
         <v>1.5680000000000001E-11</v>
       </c>
-    </row>
-    <row r="25" spans="1:9">
+      <c r="J24">
+        <f t="shared" si="0"/>
+        <v>2.2689239999999997</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
       <c r="A25">
         <v>4.0142600000000002</v>
       </c>
@@ -1227,8 +1346,12 @@
       <c r="I25" s="1">
         <v>4.089E-12</v>
       </c>
-    </row>
-    <row r="26" spans="1:9">
+      <c r="J25">
+        <f t="shared" si="0"/>
+        <v>2.4434640000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
       <c r="A26">
         <v>4.18879</v>
       </c>
@@ -1256,8 +1379,12 @@
       <c r="I26" s="1">
         <v>3.7209999999999999E-10</v>
       </c>
-    </row>
-    <row r="27" spans="1:9">
+      <c r="J26">
+        <f t="shared" si="0"/>
+        <v>2.6179939999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
       <c r="A27">
         <v>4.3633199999999999</v>
       </c>
@@ -1285,8 +1412,12 @@
       <c r="I27" s="1">
         <v>1.448E-11</v>
       </c>
-    </row>
-    <row r="28" spans="1:9">
+      <c r="J27">
+        <f t="shared" si="0"/>
+        <v>2.7925239999999998</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
       <c r="A28">
         <v>4.5378600000000002</v>
       </c>
@@ -1314,8 +1445,12 @@
       <c r="I28" s="1">
         <v>4.9490000000000002E-10</v>
       </c>
-    </row>
-    <row r="29" spans="1:9">
+      <c r="J28">
+        <f t="shared" si="0"/>
+        <v>2.9670640000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
       <c r="A29">
         <v>4.7123900000000001</v>
       </c>
@@ -1343,8 +1478,12 @@
       <c r="I29" s="1">
         <v>1.9369999999999999E-10</v>
       </c>
-    </row>
-    <row r="30" spans="1:9">
+      <c r="J29">
+        <f t="shared" si="0"/>
+        <v>3.141594</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
       <c r="A30">
         <v>4.8869199999999999</v>
       </c>
@@ -1372,8 +1511,12 @@
       <c r="I30" s="1">
         <v>3.8649999999999997E-11</v>
       </c>
-    </row>
-    <row r="31" spans="1:9">
+      <c r="J30">
+        <f t="shared" si="0"/>
+        <v>3.3161239999999998</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
       <c r="A31">
         <v>5.0614499999999998</v>
       </c>
@@ -1401,8 +1544,12 @@
       <c r="I31" s="1">
         <v>2.0339999999999999E-10</v>
       </c>
-    </row>
-    <row r="32" spans="1:9">
+      <c r="J31">
+        <f t="shared" si="0"/>
+        <v>3.4906539999999997</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
       <c r="A32">
         <v>5.2359900000000001</v>
       </c>
@@ -1430,8 +1577,12 @@
       <c r="I32" s="1">
         <v>3.3339999999999998E-11</v>
       </c>
-    </row>
-    <row r="33" spans="1:9">
+      <c r="J32">
+        <f t="shared" si="0"/>
+        <v>3.6651940000000001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
       <c r="A33">
         <v>5.41052</v>
       </c>
@@ -1459,8 +1610,12 @@
       <c r="I33" s="1">
         <v>9.3340000000000004E-13</v>
       </c>
-    </row>
-    <row r="34" spans="1:9">
+      <c r="J33">
+        <f t="shared" si="0"/>
+        <v>3.8397239999999999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
       <c r="A34">
         <v>5.5850499999999998</v>
       </c>
@@ -1488,8 +1643,12 @@
       <c r="I34" s="1">
         <v>5.325E-12</v>
       </c>
-    </row>
-    <row r="35" spans="1:9">
+      <c r="J34">
+        <f t="shared" si="0"/>
+        <v>4.0142539999999993</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
       <c r="A35">
         <v>5.7595900000000002</v>
       </c>
@@ -1517,8 +1676,12 @@
       <c r="I35" s="1">
         <v>6.64E-12</v>
       </c>
-    </row>
-    <row r="36" spans="1:9">
+      <c r="J35">
+        <f t="shared" si="0"/>
+        <v>4.1887939999999997</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10">
       <c r="A36">
         <v>5.9341200000000001</v>
       </c>
@@ -1546,8 +1709,12 @@
       <c r="I36" s="1">
         <v>7.8750000000000003E-12</v>
       </c>
-    </row>
-    <row r="37" spans="1:9">
+      <c r="J36">
+        <f t="shared" si="0"/>
+        <v>4.3633240000000004</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
       <c r="A37">
         <v>6.1086499999999999</v>
       </c>
@@ -1574,6 +1741,10 @@
       </c>
       <c r="I37" s="1">
         <v>3.1229999999999999E-13</v>
+      </c>
+      <c r="J37">
+        <f t="shared" si="0"/>
+        <v>4.5378539999999994</v>
       </c>
     </row>
   </sheetData>
@@ -1588,10 +1759,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1600,12 +1771,12 @@
     <col min="2" max="2" width="17.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1613,7 +1784,7 @@
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="D2" t="s">
         <v>12</v>
@@ -1622,13 +1793,19 @@
         <v>16</v>
       </c>
       <c r="F2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" t="s">
         <v>17</v>
       </c>
-      <c r="G2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="H2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3">
         <v>0</v>
       </c>
@@ -1650,8 +1827,14 @@
       <c r="G3">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4">
         <v>2.1999999999999999E-2</v>
       </c>
@@ -1673,8 +1856,14 @@
       <c r="G4">
         <v>1.4E-3</v>
       </c>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="H4">
+        <v>10.6</v>
+      </c>
+      <c r="I4">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5">
         <v>4.07E-2</v>
       </c>
@@ -1696,8 +1885,14 @@
       <c r="G5">
         <v>1.2999999999999999E-3</v>
       </c>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="H5">
+        <v>21.2</v>
+      </c>
+      <c r="I5">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6">
         <v>6.3899999999999998E-2</v>
       </c>
@@ -1719,8 +1914,44 @@
       <c r="G6">
         <v>1.5E-3</v>
       </c>
+      <c r="H6">
+        <v>31.8</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="H8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="H9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="H9:J12"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
@@ -1743,7 +1974,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
added field to excel
</commit_message>
<xml_diff>
--- a/Faraday Lab data tables.xlsx
+++ b/Faraday Lab data tables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1380" yWindow="460" windowWidth="19140" windowHeight="16140" tabRatio="500"/>
+    <workbookView xWindow="2520" yWindow="800" windowWidth="30480" windowHeight="17540" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ChangeThetaRaw" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
   <si>
     <t>Theta rel</t>
   </si>
@@ -56,15 +56,9 @@
     <t>Error Phase Shfit</t>
   </si>
   <si>
-    <t>B*L</t>
-  </si>
-  <si>
     <t>d(B*L)</t>
   </si>
   <si>
-    <t>V</t>
-  </si>
-  <si>
     <t>dV</t>
   </si>
   <si>
@@ -99,6 +93,12 @@
   </si>
   <si>
     <t>Theta rel actual (rad)</t>
+  </si>
+  <si>
+    <t>B*L (mT*cm)</t>
+  </si>
+  <si>
+    <t>V (V)</t>
   </si>
 </sst>
 </file>
@@ -147,8 +147,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -169,19 +171,21 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -518,7 +522,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
@@ -556,7 +560,7 @@
         <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -1762,7 +1766,7 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="H2" sqref="H2:I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1773,7 +1777,7 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -1784,25 +1788,25 @@
         <v>10</v>
       </c>
       <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" t="s">
         <v>20</v>
       </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>17</v>
-      </c>
-      <c r="H2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -1923,12 +1927,12 @@
     </row>
     <row r="8" spans="1:10">
       <c r="H8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:10">
       <c r="H9" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
@@ -1964,32 +1968,41 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="13.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" t="s">
         <v>11</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" t="s">
         <v>12</v>
       </c>
-      <c r="D1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>-3</v>
       </c>
@@ -2005,8 +2018,14 @@
       <c r="E2" s="1">
         <v>1.296E-10</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2">
+        <v>-31.8</v>
+      </c>
+      <c r="G2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>-2.5</v>
       </c>
@@ -2022,8 +2041,15 @@
       <c r="E3" s="1">
         <v>5.4699999999999997E-10</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="F3">
+        <f>AVERAGE(F2,F4)</f>
+        <v>-26.5</v>
+      </c>
+      <c r="G3">
+        <v>-0.9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>-2</v>
       </c>
@@ -2039,8 +2065,14 @@
       <c r="E4" s="1">
         <v>3.7220000000000002E-10</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="F4">
+        <v>-21.2</v>
+      </c>
+      <c r="G4">
+        <v>-0.7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>-1.5</v>
       </c>
@@ -2056,8 +2088,16 @@
       <c r="E5" s="1">
         <v>3.7749999999999999E-11</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="F5">
+        <f>AVERAGE(F4,F6)</f>
+        <v>-15.899999999999999</v>
+      </c>
+      <c r="G5">
+        <f>AVERAGE(G4,G6)</f>
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>-1</v>
       </c>
@@ -2073,8 +2113,14 @@
       <c r="E6" s="1">
         <v>8.98E-10</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="F6">
+        <v>-10.6</v>
+      </c>
+      <c r="G6">
+        <v>-0.3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>-0.5</v>
       </c>
@@ -2090,8 +2136,16 @@
       <c r="E7" s="1">
         <v>9.034E-10</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="F7">
+        <f>AVERAGE(F6,F8)</f>
+        <v>-5.3</v>
+      </c>
+      <c r="G7">
+        <f>AVERAGE(G6,G8)</f>
+        <v>-0.15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>0</v>
       </c>
@@ -2107,8 +2161,14 @@
       <c r="E8" s="1">
         <v>1.184E-9</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9">
         <v>0.5</v>
       </c>
@@ -2124,8 +2184,16 @@
       <c r="E9" s="1">
         <v>1.161E-10</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="F9">
+        <f>AVERAGE(F8,F10)</f>
+        <v>5.3</v>
+      </c>
+      <c r="G9">
+        <f>AVERAGE(G8,G10)</f>
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10">
         <v>1</v>
       </c>
@@ -2141,8 +2209,14 @@
       <c r="E10" s="1">
         <v>2.0510000000000001E-9</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="F10">
+        <v>10.6</v>
+      </c>
+      <c r="G10">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11">
         <v>1.5</v>
       </c>
@@ -2158,8 +2232,16 @@
       <c r="E11" s="1">
         <v>2.133E-9</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="F11">
+        <f>AVERAGE(F10,F12)</f>
+        <v>15.899999999999999</v>
+      </c>
+      <c r="G11">
+        <f>AVERAGE(G10,G12)</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12">
         <v>2</v>
       </c>
@@ -2175,8 +2257,14 @@
       <c r="E12" s="1">
         <v>6.9580000000000002E-10</v>
       </c>
-    </row>
-    <row r="13" spans="1:5">
+      <c r="F12">
+        <v>21.2</v>
+      </c>
+      <c r="G12">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13">
         <v>2.5</v>
       </c>
@@ -2192,8 +2280,15 @@
       <c r="E13" s="1">
         <v>1.1160000000000001E-9</v>
       </c>
-    </row>
-    <row r="14" spans="1:5">
+      <c r="F13">
+        <f>AVERAGE(F12,F14)</f>
+        <v>26.5</v>
+      </c>
+      <c r="G13">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14">
         <v>3</v>
       </c>
@@ -2208,6 +2303,12 @@
       </c>
       <c r="E14" s="1">
         <v>1.045E-9</v>
+      </c>
+      <c r="F14">
+        <v>31.8</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New error in voltage
</commit_message>
<xml_diff>
--- a/Faraday Lab data tables.xlsx
+++ b/Faraday Lab data tables.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
   <si>
     <t>Theta rel</t>
   </si>
@@ -99,6 +99,33 @@
   </si>
   <si>
     <t>V (V)</t>
+  </si>
+  <si>
+    <t>Uncertainty in V due to uncertainty in Theta:</t>
+  </si>
+  <si>
+    <t>6.2845 V/rad</t>
+  </si>
+  <si>
+    <t>dV/dTheta = -A =</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(dV/dTheta)*dTheta = </t>
+  </si>
+  <si>
+    <t>Total uncertainty in V is the sum of the computer's reported uncertainty and the propogated uncertainty from the uncertainty in angle</t>
+  </si>
+  <si>
+    <t>dV actual (V)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dTheta = 0.5deg = </t>
+  </si>
+  <si>
+    <t>0.0087 rad</t>
+  </si>
+  <si>
+    <t>0.05V</t>
   </si>
 </sst>
 </file>
@@ -147,7 +174,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -163,15 +190,21 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -179,6 +212,7 @@
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -186,6 +220,7 @@
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1968,18 +2003,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="13.1640625" customWidth="1"/>
+    <col min="9" max="9" width="24.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -2001,8 +2037,14 @@
       <c r="G1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="I1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2">
         <v>-3</v>
       </c>
@@ -2024,8 +2066,18 @@
       <c r="G2">
         <v>-1</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="I2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L2" s="4">
+        <f>E2+0.05</f>
+        <v>5.00000001296E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3">
         <v>-2.5</v>
       </c>
@@ -2048,8 +2100,18 @@
       <c r="G3">
         <v>-0.9</v>
       </c>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="I3" t="s">
+        <v>32</v>
+      </c>
+      <c r="J3" t="s">
+        <v>33</v>
+      </c>
+      <c r="L3" s="4">
+        <f t="shared" ref="L3:L14" si="0">E3+0.05</f>
+        <v>5.0000000547000004E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4">
         <v>-2</v>
       </c>
@@ -2071,8 +2133,18 @@
       <c r="G4">
         <v>-0.7</v>
       </c>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="I4" t="s">
+        <v>29</v>
+      </c>
+      <c r="J4" t="s">
+        <v>34</v>
+      </c>
+      <c r="L4" s="4">
+        <f t="shared" si="0"/>
+        <v>5.0000000372200003E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5">
         <v>-1.5</v>
       </c>
@@ -2096,8 +2168,12 @@
         <f>AVERAGE(G4,G6)</f>
         <v>-0.5</v>
       </c>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="L5" s="4">
+        <f t="shared" si="0"/>
+        <v>5.000000003775E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6">
         <v>-1</v>
       </c>
@@ -2119,8 +2195,16 @@
       <c r="G6">
         <v>-0.3</v>
       </c>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="I6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J6" s="3"/>
+      <c r="L6" s="4">
+        <f t="shared" si="0"/>
+        <v>5.0000000898000004E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7">
         <v>-0.5</v>
       </c>
@@ -2144,8 +2228,14 @@
         <f>AVERAGE(G6,G8)</f>
         <v>-0.15</v>
       </c>
-    </row>
-    <row r="8" spans="1:7">
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="L7" s="4">
+        <f t="shared" si="0"/>
+        <v>5.0000000903400003E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8">
         <v>0</v>
       </c>
@@ -2167,8 +2257,14 @@
       <c r="G8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:7">
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="L8" s="4">
+        <f t="shared" si="0"/>
+        <v>5.0000001184000005E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9">
         <v>0.5</v>
       </c>
@@ -2192,8 +2288,14 @@
         <f>AVERAGE(G8,G10)</f>
         <v>0.15</v>
       </c>
-    </row>
-    <row r="10" spans="1:7">
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="L9" s="4">
+        <f t="shared" si="0"/>
+        <v>5.00000001161E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10">
         <v>1</v>
       </c>
@@ -2215,8 +2317,14 @@
       <c r="G10">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="11" spans="1:7">
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="L10" s="4">
+        <f t="shared" si="0"/>
+        <v>5.0000002051000005E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11">
         <v>1.5</v>
       </c>
@@ -2240,8 +2348,14 @@
         <f>AVERAGE(G10,G12)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="12" spans="1:7">
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="L11" s="4">
+        <f t="shared" si="0"/>
+        <v>5.0000002133000002E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
       <c r="A12">
         <v>2</v>
       </c>
@@ -2263,8 +2377,12 @@
       <c r="G12">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="13" spans="1:7">
+      <c r="L12" s="4">
+        <f t="shared" si="0"/>
+        <v>5.0000000695800004E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
       <c r="A13">
         <v>2.5</v>
       </c>
@@ -2287,8 +2405,12 @@
       <c r="G13">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="14" spans="1:7">
+      <c r="L13" s="4">
+        <f t="shared" si="0"/>
+        <v>5.0000001116000004E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
       <c r="A14">
         <v>3</v>
       </c>
@@ -2310,9 +2432,17 @@
       <c r="G14">
         <v>1</v>
       </c>
+      <c r="L14" s="4">
+        <f t="shared" si="0"/>
+        <v>5.0000001045000006E-2</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="I6:J11"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>